<commit_message>
Remake buketservice with the confirm Order
</commit_message>
<xml_diff>
--- a/WebApplication14/wwwroot/e39e0e7b-549b-4f9c-8bb0-54dd18386a51.xlsx
+++ b/WebApplication14/wwwroot/e39e0e7b-549b-4f9c-8bb0-54dd18386a51.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -30,6 +30,15 @@
   </si>
   <si>
     <t>TotalCost</t>
+  </si>
+  <si>
+    <t>Esperanza eh144w</t>
+  </si>
+  <si>
+    <t>Headphones</t>
+  </si>
+  <si>
+    <t>Germany</t>
   </si>
 </sst>
 </file>
@@ -75,7 +84,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -102,8 +111,28 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0">
+        <v>21</v>
+      </c>
+      <c r="E2" s="0">
+        <v>40</v>
+      </c>
       <c r="F2" s="0">
-        <v>0</v>
+        <v>840</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="F3" s="0">
+        <v>840</v>
       </c>
     </row>
   </sheetData>

</xml_diff>